<commit_message>
Quinto Commit/Espero esta sea ya la version Final para lanzar
</commit_message>
<xml_diff>
--- a/corte_semanal_2025-10-23.xlsx
+++ b/corte_semanal_2025-10-23.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$9,591.40</t>
+          <t>$8.06</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$9,591.40</t>
+          <t>$8.06</t>
         </is>
       </c>
     </row>
@@ -567,10 +567,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1190</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>9591.400000000001</v>
+        <v>8.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>